<commit_message>
v2.7 now with proper timing. Still slow
</commit_message>
<xml_diff>
--- a/client/outputNN.xlsx
+++ b/client/outputNN.xlsx
@@ -877,7 +877,7 @@
         <v>471</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>36527.42056712963</v>
+        <v>36527.42068287037</v>
       </c>
       <c r="E23" t="n">
         <v>3</v>
@@ -899,7 +899,7 @@
         <v>471</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>36527.42056712963</v>
+        <v>36527.42068287037</v>
       </c>
       <c r="E24" t="n">
         <v>1</v>
@@ -943,7 +943,7 @@
         <v>470</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>36527.40003472222</v>
+        <v>36527.40024305556</v>
       </c>
       <c r="E26" t="n">
         <v>3</v>
@@ -965,7 +965,7 @@
         <v>470</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>36527.40003472222</v>
+        <v>36527.40024305556</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -1009,7 +1009,7 @@
         <v>473</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>36527.50752314815</v>
+        <v>36527.50796296296</v>
       </c>
       <c r="E29" t="n">
         <v>3</v>
@@ -1031,7 +1031,7 @@
         <v>473</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>36527.50752314815</v>
+        <v>36527.50796296296</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
@@ -1075,7 +1075,7 @@
         <v>477</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>36527.44408564815</v>
+        <v>36527.44458333333</v>
       </c>
       <c r="E32" t="n">
         <v>3</v>
@@ -1097,7 +1097,7 @@
         <v>477</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>36527.44408564815</v>
+        <v>36527.44458333333</v>
       </c>
       <c r="E33" t="n">
         <v>1</v>
@@ -1141,7 +1141,7 @@
         <v>479</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>36527.56407407407</v>
+        <v>36527.56471064815</v>
       </c>
       <c r="E35" t="n">
         <v>3</v>
@@ -1163,7 +1163,7 @@
         <v>479</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>36527.56407407407</v>
+        <v>36527.56471064815</v>
       </c>
       <c r="E36" t="n">
         <v>1</v>
@@ -1185,7 +1185,7 @@
         <v>470</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>36527.40003472222</v>
+        <v>36527.40024305556</v>
       </c>
       <c r="E37" t="n">
         <v>2</v>
@@ -1207,7 +1207,7 @@
         <v>470</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>36527.44517361111</v>
+        <v>36527.44587962963</v>
       </c>
       <c r="E38" t="n">
         <v>3</v>
@@ -1229,7 +1229,7 @@
         <v>470</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>36527.44517361111</v>
+        <v>36527.44587962963</v>
       </c>
       <c r="E39" t="n">
         <v>1</v>
@@ -1273,7 +1273,7 @@
         <v>469</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>36527.49956018518</v>
+        <v>36527.49969907408</v>
       </c>
       <c r="E41" t="n">
         <v>3</v>
@@ -1295,7 +1295,7 @@
         <v>469</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>36527.49956018518</v>
+        <v>36527.49969907408</v>
       </c>
       <c r="E42" t="n">
         <v>1</v>
@@ -1317,7 +1317,7 @@
         <v>477</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>36527.44408564815</v>
+        <v>36527.44458333333</v>
       </c>
       <c r="E43" t="n">
         <v>2</v>
@@ -1339,7 +1339,7 @@
         <v>477</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>36527.49964120371</v>
+        <v>36527.5003125</v>
       </c>
       <c r="E44" t="n">
         <v>3</v>
@@ -1361,7 +1361,7 @@
         <v>477</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>36527.49964120371</v>
+        <v>36527.5003125</v>
       </c>
       <c r="E45" t="n">
         <v>1</v>
@@ -1383,7 +1383,7 @@
         <v>470</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>36527.44517361111</v>
+        <v>36527.44587962963</v>
       </c>
       <c r="E46" t="n">
         <v>2</v>
@@ -1405,7 +1405,7 @@
         <v>470</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>36527.4903125</v>
+        <v>36527.49115740741</v>
       </c>
       <c r="E47" t="n">
         <v>3</v>
@@ -1427,7 +1427,7 @@
         <v>470</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>36527.4903125</v>
+        <v>36527.49115740741</v>
       </c>
       <c r="E48" t="n">
         <v>1</v>
@@ -1471,7 +1471,7 @@
         <v>468</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>36527.60986111111</v>
+        <v>36527.60994212963</v>
       </c>
       <c r="E50" t="n">
         <v>3</v>
@@ -1493,7 +1493,7 @@
         <v>468</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>36527.60986111111</v>
+        <v>36527.60994212963</v>
       </c>
       <c r="E51" t="n">
         <v>1</v>
@@ -1515,7 +1515,7 @@
         <v>470</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>36527.4903125</v>
+        <v>36527.49115740741</v>
       </c>
       <c r="E52" t="n">
         <v>2</v>
@@ -1537,7 +1537,7 @@
         <v>470</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>36527.54170138889</v>
+        <v>36527.54274305556</v>
       </c>
       <c r="E53" t="n">
         <v>3</v>
@@ -1559,7 +1559,7 @@
         <v>470</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>36527.54170138889</v>
+        <v>36527.54274305556</v>
       </c>
       <c r="E54" t="n">
         <v>1</v>
@@ -1603,7 +1603,7 @@
         <v>481</v>
       </c>
       <c r="D56" s="2" t="n">
-        <v>36527.5880787037</v>
+        <v>36527.58833333333</v>
       </c>
       <c r="E56" t="n">
         <v>3</v>
@@ -1625,7 +1625,7 @@
         <v>481</v>
       </c>
       <c r="D57" s="2" t="n">
-        <v>36527.5880787037</v>
+        <v>36527.58833333333</v>
       </c>
       <c r="E57" t="n">
         <v>1</v>
@@ -1647,7 +1647,7 @@
         <v>484</v>
       </c>
       <c r="D58" s="2" t="n">
-        <v>36527.49956018518</v>
+        <v>36527.49969907408</v>
       </c>
       <c r="E58" t="n">
         <v>2</v>
@@ -1669,7 +1669,7 @@
         <v>484</v>
       </c>
       <c r="D59" s="2" t="n">
-        <v>36527.54261574074</v>
+        <v>36527.54318287037</v>
       </c>
       <c r="E59" t="n">
         <v>3</v>
@@ -1691,7 +1691,7 @@
         <v>484</v>
       </c>
       <c r="D60" s="2" t="n">
-        <v>36527.54261574074</v>
+        <v>36527.54318287037</v>
       </c>
       <c r="E60" t="n">
         <v>1</v>
@@ -1713,7 +1713,7 @@
         <v>477</v>
       </c>
       <c r="D61" s="2" t="n">
-        <v>36527.49964120371</v>
+        <v>36527.5003125</v>
       </c>
       <c r="E61" t="n">
         <v>2</v>
@@ -1735,7 +1735,7 @@
         <v>477</v>
       </c>
       <c r="D62" s="2" t="n">
-        <v>36527.56283564815</v>
+        <v>36527.56415509259</v>
       </c>
       <c r="E62" t="n">
         <v>3</v>
@@ -1757,7 +1757,7 @@
         <v>477</v>
       </c>
       <c r="D63" s="2" t="n">
-        <v>36527.56283564815</v>
+        <v>36527.56415509259</v>
       </c>
       <c r="E63" t="n">
         <v>1</v>
@@ -1779,7 +1779,7 @@
         <v>476</v>
       </c>
       <c r="D64" s="2" t="n">
-        <v>36527.50752314815</v>
+        <v>36527.50796296296</v>
       </c>
       <c r="E64" t="n">
         <v>2</v>
@@ -1801,7 +1801,7 @@
         <v>476</v>
       </c>
       <c r="D65" s="2" t="n">
-        <v>36527.57210648148</v>
+        <v>36527.57296296296</v>
       </c>
       <c r="E65" t="n">
         <v>3</v>
@@ -1823,7 +1823,7 @@
         <v>476</v>
       </c>
       <c r="D66" s="2" t="n">
-        <v>36527.57210648148</v>
+        <v>36527.57296296296</v>
       </c>
       <c r="E66" t="n">
         <v>1</v>
@@ -1845,7 +1845,7 @@
         <v>473</v>
       </c>
       <c r="D67" s="2" t="n">
-        <v>36527.50752314815</v>
+        <v>36527.50796296296</v>
       </c>
       <c r="E67" t="n">
         <v>2</v>
@@ -1867,7 +1867,7 @@
         <v>473</v>
       </c>
       <c r="D68" s="2" t="n">
-        <v>36527.66724537037</v>
+        <v>36527.6682175926</v>
       </c>
       <c r="E68" t="n">
         <v>3</v>
@@ -1889,7 +1889,7 @@
         <v>473</v>
       </c>
       <c r="D69" s="2" t="n">
-        <v>36527.66724537037</v>
+        <v>36527.6682175926</v>
       </c>
       <c r="E69" t="n">
         <v>1</v>
@@ -1933,7 +1933,7 @@
         <v>472</v>
       </c>
       <c r="D71" s="2" t="n">
-        <v>36527.70388888889</v>
+        <v>36527.70394675926</v>
       </c>
       <c r="E71" t="n">
         <v>3</v>
@@ -1955,7 +1955,7 @@
         <v>472</v>
       </c>
       <c r="D72" s="2" t="n">
-        <v>36527.70388888889</v>
+        <v>36527.70394675926</v>
       </c>
       <c r="E72" t="n">
         <v>1</v>
@@ -1977,7 +1977,7 @@
         <v>483</v>
       </c>
       <c r="D73" s="2" t="n">
-        <v>36527.54261574074</v>
+        <v>36527.54318287037</v>
       </c>
       <c r="E73" t="n">
         <v>2</v>
@@ -1999,7 +1999,7 @@
         <v>483</v>
       </c>
       <c r="D74" s="2" t="n">
-        <v>36527.7780324074</v>
+        <v>36527.77878472222</v>
       </c>
       <c r="E74" t="n">
         <v>3</v>
@@ -2021,7 +2021,7 @@
         <v>483</v>
       </c>
       <c r="D75" s="2" t="n">
-        <v>36527.7780324074</v>
+        <v>36527.77878472222</v>
       </c>
       <c r="E75" t="n">
         <v>1</v>
@@ -2033,17 +2033,17 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>484_20</t>
+          <t>482_10</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C76" t="n">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D76" s="2" t="n">
-        <v>36527.56283564815</v>
+        <v>36527.56313657408</v>
       </c>
       <c r="E76" t="n">
         <v>2</v>
@@ -2055,17 +2055,17 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>484_20</t>
+          <t>482_10</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C77" t="n">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D77" s="2" t="n">
-        <v>36527.60936342592</v>
+        <v>36527.67248842592</v>
       </c>
       <c r="E77" t="n">
         <v>3</v>
@@ -2077,17 +2077,17 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>484_30</t>
+          <t>482_20</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C78" t="n">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D78" s="2" t="n">
-        <v>36527.60936342592</v>
+        <v>36527.67248842592</v>
       </c>
       <c r="E78" t="n">
         <v>1</v>
@@ -2099,17 +2099,17 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>482_10</t>
+          <t>484_20</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C79" t="n">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D79" s="2" t="n">
-        <v>36527.56313657408</v>
+        <v>36527.56415509259</v>
       </c>
       <c r="E79" t="n">
         <v>2</v>
@@ -2121,17 +2121,17 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>482_10</t>
+          <t>484_20</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C80" t="n">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D80" s="2" t="n">
-        <v>36527.67216435185</v>
+        <v>36527.61104166666</v>
       </c>
       <c r="E80" t="n">
         <v>3</v>
@@ -2143,17 +2143,17 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>482_20</t>
+          <t>484_30</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C81" t="n">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D81" s="2" t="n">
-        <v>36527.67216435185</v>
+        <v>36527.61104166666</v>
       </c>
       <c r="E81" t="n">
         <v>1</v>
@@ -2175,7 +2175,7 @@
         <v>471</v>
       </c>
       <c r="D82" s="2" t="n">
-        <v>36527.56407407407</v>
+        <v>36527.56471064815</v>
       </c>
       <c r="E82" t="n">
         <v>2</v>
@@ -2197,7 +2197,7 @@
         <v>471</v>
       </c>
       <c r="D83" s="2" t="n">
-        <v>36527.70921296296</v>
+        <v>36527.71052083333</v>
       </c>
       <c r="E83" t="n">
         <v>3</v>
@@ -2219,7 +2219,7 @@
         <v>471</v>
       </c>
       <c r="D84" s="2" t="n">
-        <v>36527.70921296296</v>
+        <v>36527.71052083333</v>
       </c>
       <c r="E84" t="n">
         <v>1</v>
@@ -2241,7 +2241,7 @@
         <v>480</v>
       </c>
       <c r="D85" s="2" t="n">
-        <v>36527.57210648148</v>
+        <v>36527.57296296296</v>
       </c>
       <c r="E85" t="n">
         <v>2</v>
@@ -2263,7 +2263,7 @@
         <v>480</v>
       </c>
       <c r="D86" s="2" t="n">
-        <v>36527.69571759259</v>
+        <v>36527.69681712963</v>
       </c>
       <c r="E86" t="n">
         <v>3</v>
@@ -2285,7 +2285,7 @@
         <v>480</v>
       </c>
       <c r="D87" s="2" t="n">
-        <v>36527.69571759259</v>
+        <v>36527.69681712963</v>
       </c>
       <c r="E87" t="n">
         <v>1</v>
@@ -2307,7 +2307,7 @@
         <v>479</v>
       </c>
       <c r="D88" s="2" t="n">
-        <v>36527.5880787037</v>
+        <v>36527.58833333333</v>
       </c>
       <c r="E88" t="n">
         <v>2</v>
@@ -2329,7 +2329,7 @@
         <v>479</v>
       </c>
       <c r="D89" s="2" t="n">
-        <v>36527.6880787037</v>
+        <v>36527.68871527778</v>
       </c>
       <c r="E89" t="n">
         <v>3</v>
@@ -2351,7 +2351,7 @@
         <v>479</v>
       </c>
       <c r="D90" s="2" t="n">
-        <v>36527.6880787037</v>
+        <v>36527.68871527778</v>
       </c>
       <c r="E90" t="n">
         <v>1</v>
@@ -2373,7 +2373,7 @@
         <v>485</v>
       </c>
       <c r="D91" s="2" t="n">
-        <v>36527.60986111111</v>
+        <v>36527.60994212963</v>
       </c>
       <c r="E91" t="n">
         <v>2</v>
@@ -2395,7 +2395,7 @@
         <v>485</v>
       </c>
       <c r="D92" s="2" t="n">
-        <v>36527.67236111111</v>
+        <v>36527.67293981482</v>
       </c>
       <c r="E92" t="n">
         <v>3</v>
@@ -2417,7 +2417,7 @@
         <v>485</v>
       </c>
       <c r="D93" s="2" t="n">
-        <v>36527.67236111111</v>
+        <v>36527.67293981482</v>
       </c>
       <c r="E93" t="n">
         <v>1</v>
@@ -2439,7 +2439,7 @@
         <v>476</v>
       </c>
       <c r="D94" s="2" t="n">
-        <v>36527.66724537037</v>
+        <v>36527.6682175926</v>
       </c>
       <c r="E94" t="n">
         <v>2</v>
@@ -2461,7 +2461,7 @@
         <v>476</v>
       </c>
       <c r="D95" s="2" t="n">
-        <v>36527.72280092593</v>
+        <v>36527.72407407407</v>
       </c>
       <c r="E95" t="n">
         <v>3</v>
@@ -2483,7 +2483,7 @@
         <v>476</v>
       </c>
       <c r="D96" s="2" t="n">
-        <v>36527.72280092593</v>
+        <v>36527.72407407407</v>
       </c>
       <c r="E96" t="n">
         <v>1</v>
@@ -2505,7 +2505,7 @@
         <v>469</v>
       </c>
       <c r="D97" s="2" t="n">
-        <v>36527.67236111111</v>
+        <v>36527.67293981482</v>
       </c>
       <c r="E97" t="n">
         <v>2</v>
@@ -2527,7 +2527,7 @@
         <v>469</v>
       </c>
       <c r="D98" s="2" t="n">
-        <v>36527.78416666666</v>
+        <v>36527.78498842593</v>
       </c>
       <c r="E98" t="n">
         <v>3</v>
@@ -2549,7 +2549,7 @@
         <v>469</v>
       </c>
       <c r="D99" s="2" t="n">
-        <v>36527.78416666666</v>
+        <v>36527.78498842593</v>
       </c>
       <c r="E99" t="n">
         <v>1</v>
@@ -2571,7 +2571,7 @@
         <v>468</v>
       </c>
       <c r="D100" s="2" t="n">
-        <v>36527.6880787037</v>
+        <v>36527.68871527778</v>
       </c>
       <c r="E100" t="n">
         <v>2</v>
@@ -2593,7 +2593,7 @@
         <v>468</v>
       </c>
       <c r="D101" s="2" t="n">
-        <v>36527.74780092593</v>
+        <v>36527.74846064814</v>
       </c>
       <c r="E101" t="n">
         <v>3</v>
@@ -2615,7 +2615,7 @@
         <v>468</v>
       </c>
       <c r="D102" s="2" t="n">
-        <v>36527.74780092593</v>
+        <v>36527.74846064814</v>
       </c>
       <c r="E102" t="n">
         <v>1</v>
@@ -2637,7 +2637,7 @@
         <v>480</v>
       </c>
       <c r="D103" s="2" t="n">
-        <v>36527.69571759259</v>
+        <v>36527.69681712963</v>
       </c>
       <c r="E103" t="n">
         <v>2</v>
@@ -2659,7 +2659,7 @@
         <v>480</v>
       </c>
       <c r="D104" s="2" t="n">
-        <v>36527.83530092592</v>
+        <v>36527.83697916667</v>
       </c>
       <c r="E104" t="n">
         <v>3</v>
@@ -2681,7 +2681,7 @@
         <v>480</v>
       </c>
       <c r="D105" s="2" t="n">
-        <v>36527.83530092592</v>
+        <v>36527.83697916667</v>
       </c>
       <c r="E105" t="n">
         <v>1</v>
@@ -2703,7 +2703,7 @@
         <v>474</v>
       </c>
       <c r="D106" s="2" t="n">
-        <v>36527.69571759259</v>
+        <v>36527.69681712963</v>
       </c>
       <c r="E106" t="n">
         <v>2</v>
@@ -2725,7 +2725,7 @@
         <v>474</v>
       </c>
       <c r="D107" s="2" t="n">
-        <v>36527.78738425926</v>
+        <v>36527.78909722222</v>
       </c>
       <c r="E107" t="n">
         <v>3</v>
@@ -2747,7 +2747,7 @@
         <v>474</v>
       </c>
       <c r="D108" s="2" t="n">
-        <v>36527.78738425926</v>
+        <v>36527.78909722222</v>
       </c>
       <c r="E108" t="n">
         <v>1</v>
@@ -2769,7 +2769,7 @@
         <v>477</v>
       </c>
       <c r="D109" s="2" t="n">
-        <v>36527.70388888889</v>
+        <v>36527.70394675926</v>
       </c>
       <c r="E109" t="n">
         <v>2</v>
@@ -2791,7 +2791,7 @@
         <v>477</v>
       </c>
       <c r="D110" s="2" t="n">
-        <v>36527.7525</v>
+        <v>36527.75273148148</v>
       </c>
       <c r="E110" t="n">
         <v>3</v>
@@ -2813,7 +2813,7 @@
         <v>477</v>
       </c>
       <c r="D111" s="2" t="n">
-        <v>36527.7525</v>
+        <v>36527.75273148148</v>
       </c>
       <c r="E111" t="n">
         <v>1</v>
@@ -2835,7 +2835,7 @@
         <v>487</v>
       </c>
       <c r="D112" s="2" t="n">
-        <v>36527.70921296296</v>
+        <v>36527.71052083333</v>
       </c>
       <c r="E112" t="n">
         <v>2</v>
@@ -2857,7 +2857,7 @@
         <v>487</v>
       </c>
       <c r="D113" s="2" t="n">
-        <v>36527.77726851852</v>
+        <v>36527.77864583334</v>
       </c>
       <c r="E113" t="n">
         <v>3</v>
@@ -2879,7 +2879,7 @@
         <v>487</v>
       </c>
       <c r="D114" s="2" t="n">
-        <v>36527.77726851852</v>
+        <v>36527.77864583334</v>
       </c>
       <c r="E114" t="n">
         <v>1</v>
@@ -2901,7 +2901,7 @@
         <v>482</v>
       </c>
       <c r="D115" s="2" t="n">
-        <v>36527.72280092593</v>
+        <v>36527.72407407407</v>
       </c>
       <c r="E115" t="n">
         <v>2</v>
@@ -2923,7 +2923,7 @@
         <v>482</v>
       </c>
       <c r="D116" s="2" t="n">
-        <v>36527.86168981482</v>
+        <v>36527.86305555556</v>
       </c>
       <c r="E116" t="n">
         <v>3</v>
@@ -2945,7 +2945,7 @@
         <v>482</v>
       </c>
       <c r="D117" s="2" t="n">
-        <v>36527.86168981482</v>
+        <v>36527.86305555556</v>
       </c>
       <c r="E117" t="n">
         <v>1</v>
@@ -2967,7 +2967,7 @@
         <v>476</v>
       </c>
       <c r="D118" s="2" t="n">
-        <v>36527.72280092593</v>
+        <v>36527.72407407407</v>
       </c>
       <c r="E118" t="n">
         <v>2</v>
@@ -2989,7 +2989,7 @@
         <v>476</v>
       </c>
       <c r="D119" s="2" t="n">
-        <v>36527.81516203703</v>
+        <v>36527.81657407407</v>
       </c>
       <c r="E119" t="n">
         <v>3</v>
@@ -3011,7 +3011,7 @@
         <v>476</v>
       </c>
       <c r="D120" s="2" t="n">
-        <v>36527.81516203703</v>
+        <v>36527.81657407407</v>
       </c>
       <c r="E120" t="n">
         <v>1</v>
@@ -3033,7 +3033,7 @@
         <v>475</v>
       </c>
       <c r="D121" s="2" t="n">
-        <v>36527.7525</v>
+        <v>36527.75273148148</v>
       </c>
       <c r="E121" t="n">
         <v>2</v>
@@ -3055,7 +3055,7 @@
         <v>475</v>
       </c>
       <c r="D122" s="2" t="n">
-        <v>36527.86916666666</v>
+        <v>36527.87006944444</v>
       </c>
       <c r="E122" t="n">
         <v>3</v>
@@ -3077,7 +3077,7 @@
         <v>475</v>
       </c>
       <c r="D123" s="2" t="n">
-        <v>36527.86916666666</v>
+        <v>36527.87006944444</v>
       </c>
       <c r="E123" t="n">
         <v>1</v>
@@ -3099,7 +3099,7 @@
         <v>486</v>
       </c>
       <c r="D124" s="2" t="n">
-        <v>36527.77726851852</v>
+        <v>36527.77864583334</v>
       </c>
       <c r="E124" t="n">
         <v>2</v>
@@ -3121,7 +3121,7 @@
         <v>486</v>
       </c>
       <c r="D125" s="2" t="n">
-        <v>36528.0925462963</v>
+        <v>36528.09439814815</v>
       </c>
       <c r="E125" t="n">
         <v>3</v>
@@ -3143,7 +3143,7 @@
         <v>486</v>
       </c>
       <c r="D126" s="2" t="n">
-        <v>36528.0925462963</v>
+        <v>36528.09439814815</v>
       </c>
       <c r="E126" t="n">
         <v>1</v>
@@ -3165,7 +3165,7 @@
         <v>485</v>
       </c>
       <c r="D127" s="2" t="n">
-        <v>36527.7780324074</v>
+        <v>36527.77878472222</v>
       </c>
       <c r="E127" t="n">
         <v>2</v>
@@ -3187,7 +3187,7 @@
         <v>485</v>
       </c>
       <c r="D128" s="2" t="n">
-        <v>36527.8717824074</v>
+        <v>36527.8728125</v>
       </c>
       <c r="E128" t="n">
         <v>3</v>
@@ -3209,7 +3209,7 @@
         <v>485</v>
       </c>
       <c r="D129" s="2" t="n">
-        <v>36527.8717824074</v>
+        <v>36527.8728125</v>
       </c>
       <c r="E129" t="n">
         <v>1</v>
@@ -3231,7 +3231,7 @@
         <v>470</v>
       </c>
       <c r="D130" s="2" t="n">
-        <v>36527.78416666666</v>
+        <v>36527.78498842593</v>
       </c>
       <c r="E130" t="n">
         <v>2</v>
@@ -3253,7 +3253,7 @@
         <v>470</v>
       </c>
       <c r="D131" s="2" t="n">
-        <v>36527.82097222222</v>
+        <v>36527.82225694445</v>
       </c>
       <c r="E131" t="n">
         <v>3</v>
@@ -3275,7 +3275,7 @@
         <v>478</v>
       </c>
       <c r="D132" s="2" t="n">
-        <v>36527.78738425926</v>
+        <v>36527.78909722222</v>
       </c>
       <c r="E132" t="n">
         <v>2</v>
@@ -3297,7 +3297,7 @@
         <v>478</v>
       </c>
       <c r="D133" s="2" t="n">
-        <v>36527.84502314815</v>
+        <v>36527.84721064815</v>
       </c>
       <c r="E133" t="n">
         <v>3</v>
@@ -3319,7 +3319,7 @@
         <v>478</v>
       </c>
       <c r="D134" s="2" t="n">
-        <v>36527.84502314815</v>
+        <v>36527.84721064815</v>
       </c>
       <c r="E134" t="n">
         <v>1</v>
@@ -3341,7 +3341,7 @@
         <v>484</v>
       </c>
       <c r="D135" s="2" t="n">
-        <v>36527.82097222222</v>
+        <v>36527.82225694445</v>
       </c>
       <c r="E135" t="n">
         <v>2</v>
@@ -3363,7 +3363,7 @@
         <v>484</v>
       </c>
       <c r="D136" s="2" t="n">
-        <v>36527.88625</v>
+        <v>36527.88777777777</v>
       </c>
       <c r="E136" t="n">
         <v>3</v>
@@ -3385,7 +3385,7 @@
         <v>484</v>
       </c>
       <c r="D137" s="2" t="n">
-        <v>36527.88625</v>
+        <v>36527.88777777777</v>
       </c>
       <c r="E137" t="n">
         <v>1</v>
@@ -3407,7 +3407,7 @@
         <v>480</v>
       </c>
       <c r="D138" s="2" t="n">
-        <v>36527.83530092592</v>
+        <v>36527.83697916667</v>
       </c>
       <c r="E138" t="n">
         <v>2</v>
@@ -3429,7 +3429,7 @@
         <v>480</v>
       </c>
       <c r="D139" s="2" t="n">
-        <v>36527.99780092593</v>
+        <v>36527.99967592592</v>
       </c>
       <c r="E139" t="n">
         <v>3</v>
@@ -3451,7 +3451,7 @@
         <v>480</v>
       </c>
       <c r="D140" s="2" t="n">
-        <v>36527.99780092593</v>
+        <v>36527.99967592592</v>
       </c>
       <c r="E140" t="n">
         <v>1</v>
@@ -3473,7 +3473,7 @@
         <v>473</v>
       </c>
       <c r="D141" s="2" t="n">
-        <v>36527.84502314815</v>
+        <v>36527.84721064815</v>
       </c>
       <c r="E141" t="n">
         <v>2</v>
@@ -3495,7 +3495,7 @@
         <v>473</v>
       </c>
       <c r="D142" s="2" t="n">
-        <v>36527.99710648148</v>
+        <v>36527.9997337963</v>
       </c>
       <c r="E142" t="n">
         <v>3</v>
@@ -3517,7 +3517,7 @@
         <v>473</v>
       </c>
       <c r="D143" s="2" t="n">
-        <v>36527.99710648148</v>
+        <v>36527.9997337963</v>
       </c>
       <c r="E143" t="n">
         <v>1</v>
@@ -3539,7 +3539,7 @@
         <v>479</v>
       </c>
       <c r="D144" s="2" t="n">
-        <v>36527.86916666666</v>
+        <v>36527.87006944444</v>
       </c>
       <c r="E144" t="n">
         <v>2</v>
@@ -3561,7 +3561,7 @@
         <v>479</v>
       </c>
       <c r="D145" s="2" t="n">
-        <v>36527.95597222223</v>
+        <v>36527.95703703703</v>
       </c>
       <c r="E145" t="n">
         <v>3</v>
@@ -3583,7 +3583,7 @@
         <v>479</v>
       </c>
       <c r="D146" s="2" t="n">
-        <v>36527.95597222223</v>
+        <v>36527.95703703703</v>
       </c>
       <c r="E146" t="n">
         <v>1</v>
@@ -3605,7 +3605,7 @@
         <v>468</v>
       </c>
       <c r="D147" s="2" t="n">
-        <v>36527.8717824074</v>
+        <v>36527.8728125</v>
       </c>
       <c r="E147" t="n">
         <v>2</v>
@@ -3627,7 +3627,7 @@
         <v>468</v>
       </c>
       <c r="D148" s="2" t="n">
-        <v>36528.00233796296</v>
+        <v>36528.00400462963</v>
       </c>
       <c r="E148" t="n">
         <v>3</v>
@@ -3649,7 +3649,7 @@
         <v>468</v>
       </c>
       <c r="D149" s="2" t="n">
-        <v>36528.00233796296</v>
+        <v>36528.00400462963</v>
       </c>
       <c r="E149" t="n">
         <v>1</v>
@@ -3671,7 +3671,7 @@
         <v>485</v>
       </c>
       <c r="D150" s="2" t="n">
-        <v>36527.8717824074</v>
+        <v>36527.8728125</v>
       </c>
       <c r="E150" t="n">
         <v>2</v>
@@ -3693,7 +3693,7 @@
         <v>485</v>
       </c>
       <c r="D151" s="2" t="n">
-        <v>36527.92525462963</v>
+        <v>36527.92640046297</v>
       </c>
       <c r="E151" t="n">
         <v>3</v>
@@ -3715,7 +3715,7 @@
         <v>485</v>
       </c>
       <c r="D152" s="2" t="n">
-        <v>36527.92525462963</v>
+        <v>36527.92640046297</v>
       </c>
       <c r="E152" t="n">
         <v>1</v>
@@ -3737,7 +3737,7 @@
         <v>478</v>
       </c>
       <c r="D153" s="2" t="n">
-        <v>36527.88625</v>
+        <v>36527.88777777777</v>
       </c>
       <c r="E153" t="n">
         <v>2</v>
@@ -3759,7 +3759,7 @@
         <v>478</v>
       </c>
       <c r="D154" s="2" t="n">
-        <v>36527.94805555556</v>
+        <v>36527.95010416667</v>
       </c>
       <c r="E154" t="n">
         <v>3</v>
@@ -3781,7 +3781,7 @@
         <v>478</v>
       </c>
       <c r="D155" s="2" t="n">
-        <v>36527.94805555556</v>
+        <v>36527.95010416667</v>
       </c>
       <c r="E155" t="n">
         <v>1</v>
@@ -3803,7 +3803,7 @@
         <v>478</v>
       </c>
       <c r="D156" s="2" t="n">
-        <v>36527.94805555556</v>
+        <v>36527.95010416667</v>
       </c>
       <c r="E156" t="n">
         <v>2</v>
@@ -3825,7 +3825,7 @@
         <v>478</v>
       </c>
       <c r="D157" s="2" t="n">
-        <v>36528.03694444444</v>
+        <v>36528.03921296296</v>
       </c>
       <c r="E157" t="n">
         <v>3</v>
@@ -3847,7 +3847,7 @@
         <v>478</v>
       </c>
       <c r="D158" s="2" t="n">
-        <v>36528.03694444444</v>
+        <v>36528.03921296296</v>
       </c>
       <c r="E158" t="n">
         <v>1</v>
@@ -3869,7 +3869,7 @@
         <v>485</v>
       </c>
       <c r="D159" s="2" t="n">
-        <v>36527.94805555556</v>
+        <v>36527.95010416667</v>
       </c>
       <c r="E159" t="n">
         <v>2</v>
@@ -3891,7 +3891,7 @@
         <v>485</v>
       </c>
       <c r="D160" s="2" t="n">
-        <v>36527.99805555555</v>
+        <v>36528.00060185185</v>
       </c>
       <c r="E160" t="n">
         <v>3</v>
@@ -3913,7 +3913,7 @@
         <v>485</v>
       </c>
       <c r="D161" s="2" t="n">
-        <v>36527.99805555555</v>
+        <v>36528.00060185185</v>
       </c>
       <c r="E161" t="n">
         <v>1</v>
@@ -3935,7 +3935,7 @@
         <v>483</v>
       </c>
       <c r="D162" s="2" t="n">
-        <v>36527.95597222223</v>
+        <v>36527.95703703703</v>
       </c>
       <c r="E162" t="n">
         <v>2</v>
@@ -3957,7 +3957,7 @@
         <v>483</v>
       </c>
       <c r="D163" s="2" t="n">
-        <v>36528.22472222222</v>
+        <v>36528.22615740741</v>
       </c>
       <c r="E163" t="n">
         <v>3</v>
@@ -3979,7 +3979,7 @@
         <v>483</v>
       </c>
       <c r="D164" s="2" t="n">
-        <v>36528.22472222222</v>
+        <v>36528.22615740741</v>
       </c>
       <c r="E164" t="n">
         <v>1</v>
@@ -3991,17 +3991,17 @@
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>472_20</t>
+          <t>482_30</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C165" t="n">
-        <v>472</v>
+        <v>482</v>
       </c>
       <c r="D165" s="2" t="n">
-        <v>36527.99710648148</v>
+        <v>36527.99967592592</v>
       </c>
       <c r="E165" t="n">
         <v>2</v>
@@ -4013,17 +4013,17 @@
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>472_20</t>
+          <t>482_30</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C166" t="n">
-        <v>472</v>
+        <v>482</v>
       </c>
       <c r="D166" s="2" t="n">
-        <v>36528.19432870371</v>
+        <v>36528.08840277778</v>
       </c>
       <c r="E166" t="n">
         <v>3</v>
@@ -4035,17 +4035,17 @@
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>472_30</t>
+          <t>482_40</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C167" t="n">
-        <v>472</v>
+        <v>482</v>
       </c>
       <c r="D167" s="2" t="n">
-        <v>36528.19432870371</v>
+        <v>36528.08840277778</v>
       </c>
       <c r="E167" t="n">
         <v>1</v>
@@ -4057,17 +4057,17 @@
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>473_40</t>
+          <t>472_20</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C168" t="n">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D168" s="2" t="n">
-        <v>36527.99710648148</v>
+        <v>36527.9997337963</v>
       </c>
       <c r="E168" t="n">
         <v>2</v>
@@ -4079,17 +4079,17 @@
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>473_40</t>
+          <t>472_20</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C169" t="n">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D169" s="2" t="n">
-        <v>36528.14502314815</v>
+        <v>36528.19733796296</v>
       </c>
       <c r="E169" t="n">
         <v>3</v>
@@ -4101,17 +4101,17 @@
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>473_50</t>
+          <t>472_30</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C170" t="n">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D170" s="2" t="n">
-        <v>36528.14502314815</v>
+        <v>36528.19733796296</v>
       </c>
       <c r="E170" t="n">
         <v>1</v>
@@ -4123,17 +4123,17 @@
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>482_30</t>
+          <t>473_40</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C171" t="n">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="D171" s="2" t="n">
-        <v>36527.99780092593</v>
+        <v>36527.9997337963</v>
       </c>
       <c r="E171" t="n">
         <v>2</v>
@@ -4145,17 +4145,17 @@
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>482_30</t>
+          <t>473_40</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C172" t="n">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="D172" s="2" t="n">
-        <v>36528.08599537037</v>
+        <v>36528.14805555555</v>
       </c>
       <c r="E172" t="n">
         <v>3</v>
@@ -4167,17 +4167,17 @@
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>482_40</t>
+          <t>473_50</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C173" t="n">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="D173" s="2" t="n">
-        <v>36528.08599537037</v>
+        <v>36528.14805555555</v>
       </c>
       <c r="E173" t="n">
         <v>1</v>
@@ -4199,7 +4199,7 @@
         <v>479</v>
       </c>
       <c r="D174" s="2" t="n">
-        <v>36527.99805555555</v>
+        <v>36528.00060185185</v>
       </c>
       <c r="E174" t="n">
         <v>2</v>
@@ -4221,7 +4221,7 @@
         <v>479</v>
       </c>
       <c r="D175" s="2" t="n">
-        <v>36528.09041666667</v>
+        <v>36528.093125</v>
       </c>
       <c r="E175" t="n">
         <v>3</v>
@@ -4243,7 +4243,7 @@
         <v>479</v>
       </c>
       <c r="D176" s="2" t="n">
-        <v>36528.09041666667</v>
+        <v>36528.093125</v>
       </c>
       <c r="E176" t="n">
         <v>1</v>
@@ -4265,7 +4265,7 @@
         <v>487</v>
       </c>
       <c r="D177" s="2" t="n">
-        <v>36528.00233796296</v>
+        <v>36528.00400462963</v>
       </c>
       <c r="E177" t="n">
         <v>2</v>
@@ -4287,7 +4287,7 @@
         <v>487</v>
       </c>
       <c r="D178" s="2" t="n">
-        <v>36528.08011574074</v>
+        <v>36528.08210648148</v>
       </c>
       <c r="E178" t="n">
         <v>3</v>
@@ -4309,7 +4309,7 @@
         <v>487</v>
       </c>
       <c r="D179" s="2" t="n">
-        <v>36528.08011574074</v>
+        <v>36528.08210648148</v>
       </c>
       <c r="E179" t="n">
         <v>1</v>
@@ -4331,7 +4331,7 @@
         <v>478</v>
       </c>
       <c r="D180" s="2" t="n">
-        <v>36528.03694444444</v>
+        <v>36528.03921296296</v>
       </c>
       <c r="E180" t="n">
         <v>2</v>
@@ -4353,7 +4353,7 @@
         <v>478</v>
       </c>
       <c r="D181" s="2" t="n">
-        <v>36528.09944444444</v>
+        <v>36528.10231481482</v>
       </c>
       <c r="E181" t="n">
         <v>3</v>
@@ -4375,7 +4375,7 @@
         <v>478</v>
       </c>
       <c r="D182" s="2" t="n">
-        <v>36528.09944444444</v>
+        <v>36528.10231481482</v>
       </c>
       <c r="E182" t="n">
         <v>1</v>
@@ -4397,7 +4397,7 @@
         <v>485</v>
       </c>
       <c r="D183" s="2" t="n">
-        <v>36528.08011574074</v>
+        <v>36528.08210648148</v>
       </c>
       <c r="E183" t="n">
         <v>2</v>
@@ -4419,7 +4419,7 @@
         <v>485</v>
       </c>
       <c r="D184" s="2" t="n">
-        <v>36528.14469907407</v>
+        <v>36528.14721064815</v>
       </c>
       <c r="E184" t="n">
         <v>3</v>
@@ -4441,7 +4441,7 @@
         <v>485</v>
       </c>
       <c r="D185" s="2" t="n">
-        <v>36528.14469907407</v>
+        <v>36528.14721064815</v>
       </c>
       <c r="E185" t="n">
         <v>1</v>
@@ -4463,7 +4463,7 @@
         <v>475</v>
       </c>
       <c r="D186" s="2" t="n">
-        <v>36528.08599537037</v>
+        <v>36528.08840277778</v>
       </c>
       <c r="E186" t="n">
         <v>2</v>
@@ -4485,7 +4485,7 @@
         <v>475</v>
       </c>
       <c r="D187" s="2" t="n">
-        <v>36528.17349537037</v>
+        <v>36528.1759837963</v>
       </c>
       <c r="E187" t="n">
         <v>3</v>
@@ -4507,7 +4507,7 @@
         <v>475</v>
       </c>
       <c r="D188" s="2" t="n">
-        <v>36528.17349537037</v>
+        <v>36528.1759837963</v>
       </c>
       <c r="E188" t="n">
         <v>1</v>
@@ -4529,7 +4529,7 @@
         <v>479</v>
       </c>
       <c r="D189" s="2" t="n">
-        <v>36528.09041666667</v>
+        <v>36528.093125</v>
       </c>
       <c r="E189" t="n">
         <v>2</v>
@@ -4551,7 +4551,7 @@
         <v>479</v>
       </c>
       <c r="D190" s="2" t="n">
-        <v>36528.17027777778</v>
+        <v>36528.17326388889</v>
       </c>
       <c r="E190" t="n">
         <v>3</v>
@@ -4573,7 +4573,7 @@
         <v>479</v>
       </c>
       <c r="D191" s="2" t="n">
-        <v>36528.17027777778</v>
+        <v>36528.17326388889</v>
       </c>
       <c r="E191" t="n">
         <v>1</v>
@@ -4595,7 +4595,7 @@
         <v>480</v>
       </c>
       <c r="D192" s="2" t="n">
-        <v>36528.09041666667</v>
+        <v>36528.093125</v>
       </c>
       <c r="E192" t="n">
         <v>2</v>
@@ -4617,7 +4617,7 @@
         <v>480</v>
       </c>
       <c r="D193" s="2" t="n">
-        <v>36528.255</v>
+        <v>36528.25795138889</v>
       </c>
       <c r="E193" t="n">
         <v>3</v>
@@ -4639,7 +4639,7 @@
         <v>480</v>
       </c>
       <c r="D194" s="2" t="n">
-        <v>36528.255</v>
+        <v>36528.25795138889</v>
       </c>
       <c r="E194" t="n">
         <v>1</v>
@@ -4661,7 +4661,7 @@
         <v>481</v>
       </c>
       <c r="D195" s="2" t="n">
-        <v>36528.0925462963</v>
+        <v>36528.09439814815</v>
       </c>
       <c r="E195" t="n">
         <v>2</v>
@@ -4683,7 +4683,7 @@
         <v>481</v>
       </c>
       <c r="D196" s="2" t="n">
-        <v>36528.17449074074</v>
+        <v>36528.17700231481</v>
       </c>
       <c r="E196" t="n">
         <v>3</v>
@@ -4705,7 +4705,7 @@
         <v>481</v>
       </c>
       <c r="D197" s="2" t="n">
-        <v>36528.17449074074</v>
+        <v>36528.17700231481</v>
       </c>
       <c r="E197" t="n">
         <v>1</v>
@@ -4727,7 +4727,7 @@
         <v>478</v>
       </c>
       <c r="D198" s="2" t="n">
-        <v>36528.09944444444</v>
+        <v>36528.10231481482</v>
       </c>
       <c r="E198" t="n">
         <v>2</v>
@@ -4749,7 +4749,7 @@
         <v>478</v>
       </c>
       <c r="D199" s="2" t="n">
-        <v>36528.16402777778</v>
+        <v>36528.16747685185</v>
       </c>
       <c r="E199" t="n">
         <v>3</v>
@@ -4771,7 +4771,7 @@
         <v>478</v>
       </c>
       <c r="D200" s="2" t="n">
-        <v>36528.16402777778</v>
+        <v>36528.16747685185</v>
       </c>
       <c r="E200" t="n">
         <v>1</v>
@@ -4793,7 +4793,7 @@
         <v>482</v>
       </c>
       <c r="D201" s="2" t="n">
-        <v>36528.14469907407</v>
+        <v>36528.14721064815</v>
       </c>
       <c r="E201" t="n">
         <v>2</v>
@@ -4815,7 +4815,7 @@
         <v>482</v>
       </c>
       <c r="D202" s="2" t="n">
-        <v>36528.26344907407</v>
+        <v>36528.26649305555</v>
       </c>
       <c r="E202" t="n">
         <v>3</v>
@@ -4837,7 +4837,7 @@
         <v>482</v>
       </c>
       <c r="D203" s="2" t="n">
-        <v>36528.26344907407</v>
+        <v>36528.26649305555</v>
       </c>
       <c r="E203" t="n">
         <v>1</v>
@@ -4859,7 +4859,7 @@
         <v>487</v>
       </c>
       <c r="D204" s="2" t="n">
-        <v>36528.14502314815</v>
+        <v>36528.14805555555</v>
       </c>
       <c r="E204" t="n">
         <v>2</v>
@@ -4881,7 +4881,7 @@
         <v>487</v>
       </c>
       <c r="D205" s="2" t="n">
-        <v>36528.23043981481</v>
+        <v>36528.23376157408</v>
       </c>
       <c r="E205" t="n">
         <v>3</v>
@@ -4903,7 +4903,7 @@
         <v>487</v>
       </c>
       <c r="D206" s="2" t="n">
-        <v>36528.23043981481</v>
+        <v>36528.23376157408</v>
       </c>
       <c r="E206" t="n">
         <v>1</v>
@@ -4925,7 +4925,7 @@
         <v>485</v>
       </c>
       <c r="D207" s="2" t="n">
-        <v>36528.16402777778</v>
+        <v>36528.16747685185</v>
       </c>
       <c r="E207" t="n">
         <v>2</v>
@@ -4947,7 +4947,7 @@
         <v>485</v>
       </c>
       <c r="D208" s="2" t="n">
-        <v>36528.23833333333</v>
+        <v>36528.24216435185</v>
       </c>
       <c r="E208" t="n">
         <v>3</v>
@@ -4969,7 +4969,7 @@
         <v>485</v>
       </c>
       <c r="D209" s="2" t="n">
-        <v>36528.23833333333</v>
+        <v>36528.24216435185</v>
       </c>
       <c r="E209" t="n">
         <v>1</v>
@@ -4991,7 +4991,7 @@
         <v>486</v>
       </c>
       <c r="D210" s="2" t="n">
-        <v>36528.17027777778</v>
+        <v>36528.17326388889</v>
       </c>
       <c r="E210" t="n">
         <v>2</v>
@@ -5013,7 +5013,7 @@
         <v>486</v>
       </c>
       <c r="D211" s="2" t="n">
-        <v>36528.42930555555</v>
+        <v>36528.43253472223</v>
       </c>
       <c r="E211" t="n">
         <v>3</v>
@@ -5035,7 +5035,7 @@
         <v>486</v>
       </c>
       <c r="D212" s="2" t="n">
-        <v>36528.42930555555</v>
+        <v>36528.43253472223</v>
       </c>
       <c r="E212" t="n">
         <v>1</v>
@@ -5057,7 +5057,7 @@
         <v>468</v>
       </c>
       <c r="D213" s="2" t="n">
-        <v>36528.17349537037</v>
+        <v>36528.1759837963</v>
       </c>
       <c r="E213" t="n">
         <v>2</v>
@@ -5079,7 +5079,7 @@
         <v>468</v>
       </c>
       <c r="D214" s="2" t="n">
-        <v>36528.22488425926</v>
+        <v>36528.22788194445</v>
       </c>
       <c r="E214" t="n">
         <v>3</v>
@@ -5101,7 +5101,7 @@
         <v>468</v>
       </c>
       <c r="D215" s="2" t="n">
-        <v>36528.22488425926</v>
+        <v>36528.22788194445</v>
       </c>
       <c r="E215" t="n">
         <v>1</v>
@@ -5123,7 +5123,7 @@
         <v>469</v>
       </c>
       <c r="D216" s="2" t="n">
-        <v>36528.17449074074</v>
+        <v>36528.17700231481</v>
       </c>
       <c r="E216" t="n">
         <v>2</v>
@@ -5145,7 +5145,7 @@
         <v>469</v>
       </c>
       <c r="D217" s="2" t="n">
-        <v>36528.23490740741</v>
+        <v>36528.23788194444</v>
       </c>
       <c r="E217" t="n">
         <v>3</v>
@@ -5167,7 +5167,7 @@
         <v>469</v>
       </c>
       <c r="D218" s="2" t="n">
-        <v>36528.23490740741</v>
+        <v>36528.23788194444</v>
       </c>
       <c r="E218" t="n">
         <v>1</v>
@@ -5189,7 +5189,7 @@
         <v>471</v>
       </c>
       <c r="D219" s="2" t="n">
-        <v>36528.19432870371</v>
+        <v>36528.19733796296</v>
       </c>
       <c r="E219" t="n">
         <v>2</v>
@@ -5211,7 +5211,7 @@
         <v>471</v>
       </c>
       <c r="D220" s="2" t="n">
-        <v>36528.27210648148</v>
+        <v>36528.27533564815</v>
       </c>
       <c r="E220" t="n">
         <v>3</v>
@@ -5233,7 +5233,7 @@
         <v>471</v>
       </c>
       <c r="D221" s="2" t="n">
-        <v>36528.27210648148</v>
+        <v>36528.27533564815</v>
       </c>
       <c r="E221" t="n">
         <v>1</v>
@@ -5255,7 +5255,7 @@
         <v>474</v>
       </c>
       <c r="D222" s="2" t="n">
-        <v>36528.22472222222</v>
+        <v>36528.22615740741</v>
       </c>
       <c r="E222" t="n">
         <v>2</v>
@@ -5277,7 +5277,7 @@
         <v>474</v>
       </c>
       <c r="D223" s="2" t="n">
-        <v>36528.4525</v>
+        <v>36528.45409722222</v>
       </c>
       <c r="E223" t="n">
         <v>3</v>
@@ -5299,7 +5299,7 @@
         <v>474</v>
       </c>
       <c r="D224" s="2" t="n">
-        <v>36528.4525</v>
+        <v>36528.45409722222</v>
       </c>
       <c r="E224" t="n">
         <v>1</v>
@@ -5321,7 +5321,7 @@
         <v>481</v>
       </c>
       <c r="D225" s="2" t="n">
-        <v>36528.22488425926</v>
+        <v>36528.22788194445</v>
       </c>
       <c r="E225" t="n">
         <v>2</v>
@@ -5343,7 +5343,7 @@
         <v>481</v>
       </c>
       <c r="D226" s="2" t="n">
-        <v>36528.30613425926</v>
+        <v>36528.30936342593</v>
       </c>
       <c r="E226" t="n">
         <v>3</v>
@@ -5365,7 +5365,7 @@
         <v>481</v>
       </c>
       <c r="D227" s="2" t="n">
-        <v>36528.30613425926</v>
+        <v>36528.30936342593</v>
       </c>
       <c r="E227" t="n">
         <v>1</v>
@@ -5387,7 +5387,7 @@
         <v>483</v>
       </c>
       <c r="D228" s="2" t="n">
-        <v>36528.23043981481</v>
+        <v>36528.23376157408</v>
       </c>
       <c r="E228" t="n">
         <v>2</v>
@@ -5409,7 +5409,7 @@
         <v>483</v>
       </c>
       <c r="D229" s="2" t="n">
-        <v>36528.48738425926</v>
+        <v>36528.49136574074</v>
       </c>
       <c r="E229" t="n">
         <v>3</v>
@@ -5431,7 +5431,7 @@
         <v>483</v>
       </c>
       <c r="D230" s="2" t="n">
-        <v>36528.48738425926</v>
+        <v>36528.49136574074</v>
       </c>
       <c r="E230" t="n">
         <v>1</v>
@@ -5453,7 +5453,7 @@
         <v>484</v>
       </c>
       <c r="D231" s="2" t="n">
-        <v>36528.23490740741</v>
+        <v>36528.23788194444</v>
       </c>
       <c r="E231" t="n">
         <v>2</v>
@@ -5475,7 +5475,7 @@
         <v>484</v>
       </c>
       <c r="D232" s="2" t="n">
-        <v>36528.2612962963</v>
+        <v>36528.26487268518</v>
       </c>
       <c r="E232" t="n">
         <v>3</v>
@@ -5497,7 +5497,7 @@
         <v>484</v>
       </c>
       <c r="D233" s="2" t="n">
-        <v>36528.2612962963</v>
+        <v>36528.26487268518</v>
       </c>
       <c r="E233" t="n">
         <v>1</v>
@@ -5519,7 +5519,7 @@
         <v>472</v>
       </c>
       <c r="D234" s="2" t="n">
-        <v>36528.255</v>
+        <v>36528.25795138889</v>
       </c>
       <c r="E234" t="n">
         <v>2</v>
@@ -5541,7 +5541,7 @@
         <v>472</v>
       </c>
       <c r="D235" s="2" t="n">
-        <v>36528.45986111111</v>
+        <v>36528.4628125</v>
       </c>
       <c r="E235" t="n">
         <v>3</v>
@@ -5563,7 +5563,7 @@
         <v>472</v>
       </c>
       <c r="D236" s="2" t="n">
-        <v>36528.45986111111</v>
+        <v>36528.4628125</v>
       </c>
       <c r="E236" t="n">
         <v>1</v>
@@ -5585,7 +5585,7 @@
         <v>478</v>
       </c>
       <c r="D237" s="2" t="n">
-        <v>36528.2612962963</v>
+        <v>36528.26487268518</v>
       </c>
       <c r="E237" t="n">
         <v>2</v>
@@ -5607,7 +5607,7 @@
         <v>478</v>
       </c>
       <c r="D238" s="2" t="n">
-        <v>36528.32796296296</v>
+        <v>36528.33207175926</v>
       </c>
       <c r="E238" t="n">
         <v>3</v>
@@ -5629,7 +5629,7 @@
         <v>484</v>
       </c>
       <c r="D239" s="2" t="n">
-        <v>36528.2612962963</v>
+        <v>36528.26487268518</v>
       </c>
       <c r="E239" t="n">
         <v>2</v>
@@ -5651,7 +5651,7 @@
         <v>484</v>
       </c>
       <c r="D240" s="2" t="n">
-        <v>36528.33143518519</v>
+        <v>36528.33519675926</v>
       </c>
       <c r="E240" t="n">
         <v>3</v>
@@ -5673,7 +5673,7 @@
         <v>484</v>
       </c>
       <c r="D241" s="2" t="n">
-        <v>36528.33143518519</v>
+        <v>36528.33519675926</v>
       </c>
       <c r="E241" t="n">
         <v>1</v>
@@ -5695,7 +5695,7 @@
         <v>482</v>
       </c>
       <c r="D242" s="2" t="n">
-        <v>36528.26344907407</v>
+        <v>36528.26649305555</v>
       </c>
       <c r="E242" t="n">
         <v>2</v>
@@ -5717,7 +5717,7 @@
         <v>482</v>
       </c>
       <c r="D243" s="2" t="n">
-        <v>36528.40025462963</v>
+        <v>36528.40378472222</v>
       </c>
       <c r="E243" t="n">
         <v>3</v>
@@ -5739,7 +5739,7 @@
         <v>482</v>
       </c>
       <c r="D244" s="2" t="n">
-        <v>36528.40025462963</v>
+        <v>36528.40378472222</v>
       </c>
       <c r="E244" t="n">
         <v>1</v>
@@ -5761,7 +5761,7 @@
         <v>475</v>
       </c>
       <c r="D245" s="2" t="n">
-        <v>36528.26344907407</v>
+        <v>36528.26649305555</v>
       </c>
       <c r="E245" t="n">
         <v>2</v>
@@ -5783,7 +5783,7 @@
         <v>475</v>
       </c>
       <c r="D246" s="2" t="n">
-        <v>36528.31344907408</v>
+        <v>36528.31702546297</v>
       </c>
       <c r="E246" t="n">
         <v>3</v>
@@ -5805,7 +5805,7 @@
         <v>475</v>
       </c>
       <c r="D247" s="2" t="n">
-        <v>36528.31344907408</v>
+        <v>36528.31702546297</v>
       </c>
       <c r="E247" t="n">
         <v>1</v>
@@ -5827,7 +5827,7 @@
         <v>477</v>
       </c>
       <c r="D248" s="2" t="n">
-        <v>36528.27210648148</v>
+        <v>36528.27533564815</v>
       </c>
       <c r="E248" t="n">
         <v>2</v>
@@ -5849,7 +5849,7 @@
         <v>477</v>
       </c>
       <c r="D249" s="2" t="n">
-        <v>36528.31168981481</v>
+        <v>36528.31548611111</v>
       </c>
       <c r="E249" t="n">
         <v>3</v>
@@ -5871,7 +5871,7 @@
         <v>473</v>
       </c>
       <c r="D250" s="2" t="n">
-        <v>36528.31168981481</v>
+        <v>36528.31548611111</v>
       </c>
       <c r="E250" t="n">
         <v>2</v>
@@ -5893,7 +5893,7 @@
         <v>473</v>
       </c>
       <c r="D251" s="2" t="n">
-        <v>36528.35543981481</v>
+        <v>36528.35982638889</v>
       </c>
       <c r="E251" t="n">
         <v>3</v>
@@ -5915,7 +5915,7 @@
         <v>468</v>
       </c>
       <c r="D252" s="2" t="n">
-        <v>36528.31344907408</v>
+        <v>36528.31702546297</v>
       </c>
       <c r="E252" t="n">
         <v>2</v>
@@ -5937,7 +5937,7 @@
         <v>468</v>
       </c>
       <c r="D253" s="2" t="n">
-        <v>36528.35372685185</v>
+        <v>36528.35792824074</v>
       </c>
       <c r="E253" t="n">
         <v>3</v>
@@ -5959,7 +5959,7 @@
         <v>485</v>
       </c>
       <c r="D254" s="2" t="n">
-        <v>36528.32796296296</v>
+        <v>36528.33207175926</v>
       </c>
       <c r="E254" t="n">
         <v>2</v>
@@ -5981,7 +5981,7 @@
         <v>485</v>
       </c>
       <c r="D255" s="2" t="n">
-        <v>36528.35365740741</v>
+        <v>36528.35791666667</v>
       </c>
       <c r="E255" t="n">
         <v>3</v>
@@ -6003,7 +6003,7 @@
         <v>481</v>
       </c>
       <c r="D256" s="2" t="n">
-        <v>36528.33143518519</v>
+        <v>36528.33519675926</v>
       </c>
       <c r="E256" t="n">
         <v>2</v>
@@ -6025,7 +6025,7 @@
         <v>481</v>
       </c>
       <c r="D257" s="2" t="n">
-        <v>36528.49532407407</v>
+        <v>36528.49974537037</v>
       </c>
       <c r="E257" t="n">
         <v>3</v>
@@ -6047,7 +6047,7 @@
         <v>481</v>
       </c>
       <c r="D258" s="2" t="n">
-        <v>36528.49532407407</v>
+        <v>36528.49974537037</v>
       </c>
       <c r="E258" t="n">
         <v>1</v>
@@ -6069,7 +6069,7 @@
         <v>487</v>
       </c>
       <c r="D259" s="2" t="n">
-        <v>36528.35372685185</v>
+        <v>36528.35792824074</v>
       </c>
       <c r="E259" t="n">
         <v>2</v>
@@ -6091,7 +6091,7 @@
         <v>487</v>
       </c>
       <c r="D260" s="2" t="n">
-        <v>36528.44539351852</v>
+        <v>36528.45009259259</v>
       </c>
       <c r="E260" t="n">
         <v>3</v>
@@ -6113,7 +6113,7 @@
         <v>479</v>
       </c>
       <c r="D261" s="2" t="n">
-        <v>36528.35543981481</v>
+        <v>36528.35982638889</v>
       </c>
       <c r="E261" t="n">
         <v>2</v>
@@ -6135,7 +6135,7 @@
         <v>479</v>
       </c>
       <c r="D262" s="2" t="n">
-        <v>36528.52141203704</v>
+        <v>36528.52600694444</v>
       </c>
       <c r="E262" t="n">
         <v>3</v>
@@ -6157,7 +6157,7 @@
         <v>469</v>
       </c>
       <c r="D263" s="2" t="n">
-        <v>36528.42930555555</v>
+        <v>36528.43253472223</v>
       </c>
       <c r="E263" t="n">
         <v>2</v>
@@ -6179,7 +6179,7 @@
         <v>469</v>
       </c>
       <c r="D264" s="2" t="n">
-        <v>36528.48208333334</v>
+        <v>36528.48545138889</v>
       </c>
       <c r="E264" t="n">
         <v>3</v>
@@ -6201,7 +6201,7 @@
         <v>469</v>
       </c>
       <c r="D265" s="2" t="n">
-        <v>36528.48208333334</v>
+        <v>36528.48545138889</v>
       </c>
       <c r="E265" t="n">
         <v>1</v>
@@ -6223,7 +6223,7 @@
         <v>482</v>
       </c>
       <c r="D266" s="2" t="n">
-        <v>36528.44539351852</v>
+        <v>36528.45009259259</v>
       </c>
       <c r="E266" t="n">
         <v>2</v>
@@ -6245,7 +6245,7 @@
         <v>482</v>
       </c>
       <c r="D267" s="2" t="n">
-        <v>36528.56136574074</v>
+        <v>36528.56638888889</v>
       </c>
       <c r="E267" t="n">
         <v>3</v>
@@ -6267,7 +6267,7 @@
         <v>476</v>
       </c>
       <c r="D268" s="2" t="n">
-        <v>36528.4525</v>
+        <v>36528.45409722222</v>
       </c>
       <c r="E268" t="n">
         <v>2</v>
@@ -6289,7 +6289,7 @@
         <v>476</v>
       </c>
       <c r="D269" s="2" t="n">
-        <v>36528.51569444445</v>
+        <v>36528.51758101852</v>
       </c>
       <c r="E269" t="n">
         <v>3</v>
@@ -6311,7 +6311,7 @@
         <v>476</v>
       </c>
       <c r="D270" s="2" t="n">
-        <v>36528.51569444445</v>
+        <v>36528.51758101852</v>
       </c>
       <c r="E270" t="n">
         <v>1</v>
@@ -6333,7 +6333,7 @@
         <v>475</v>
       </c>
       <c r="D271" s="2" t="n">
-        <v>36528.45986111111</v>
+        <v>36528.4628125</v>
       </c>
       <c r="E271" t="n">
         <v>2</v>
@@ -6355,7 +6355,7 @@
         <v>475</v>
       </c>
       <c r="D272" s="2" t="n">
-        <v>36528.58625</v>
+        <v>36528.58936342593</v>
       </c>
       <c r="E272" t="n">
         <v>3</v>
@@ -6377,7 +6377,7 @@
         <v>475</v>
       </c>
       <c r="D273" s="2" t="n">
-        <v>36528.58625</v>
+        <v>36528.58936342593</v>
       </c>
       <c r="E273" t="n">
         <v>1</v>
@@ -6399,7 +6399,7 @@
         <v>484</v>
       </c>
       <c r="D274" s="2" t="n">
-        <v>36528.48208333334</v>
+        <v>36528.48545138889</v>
       </c>
       <c r="E274" t="n">
         <v>2</v>
@@ -6421,7 +6421,7 @@
         <v>484</v>
       </c>
       <c r="D275" s="2" t="n">
-        <v>36528.50777777778</v>
+        <v>36528.51181712963</v>
       </c>
       <c r="E275" t="n">
         <v>3</v>
@@ -6443,7 +6443,7 @@
         <v>484</v>
       </c>
       <c r="D276" s="2" t="n">
-        <v>36528.50777777778</v>
+        <v>36528.51181712963</v>
       </c>
       <c r="E276" t="n">
         <v>1</v>
@@ -6465,7 +6465,7 @@
         <v>469</v>
       </c>
       <c r="D277" s="2" t="n">
-        <v>36528.48208333334</v>
+        <v>36528.48545138889</v>
       </c>
       <c r="E277" t="n">
         <v>2</v>
@@ -6487,7 +6487,7 @@
         <v>469</v>
       </c>
       <c r="D278" s="2" t="n">
-        <v>36528.58694444445</v>
+        <v>36528.59071759259</v>
       </c>
       <c r="E278" t="n">
         <v>3</v>
@@ -6509,7 +6509,7 @@
         <v>469</v>
       </c>
       <c r="D279" s="2" t="n">
-        <v>36528.58694444445</v>
+        <v>36528.59071759259</v>
       </c>
       <c r="E279" t="n">
         <v>1</v>
@@ -6531,7 +6531,7 @@
         <v>483</v>
       </c>
       <c r="D280" s="2" t="n">
-        <v>36528.48738425926</v>
+        <v>36528.49136574074</v>
       </c>
       <c r="E280" t="n">
         <v>2</v>
@@ -6553,7 +6553,7 @@
         <v>483</v>
       </c>
       <c r="D281" s="2" t="n">
-        <v>36528.72974537037</v>
+        <v>36528.73409722222</v>
       </c>
       <c r="E281" t="n">
         <v>3</v>
@@ -6575,7 +6575,7 @@
         <v>483</v>
       </c>
       <c r="D282" s="2" t="n">
-        <v>36528.72974537037</v>
+        <v>36528.73409722222</v>
       </c>
       <c r="E282" t="n">
         <v>1</v>
@@ -6597,7 +6597,7 @@
         <v>471</v>
       </c>
       <c r="D283" s="2" t="n">
-        <v>36528.51569444445</v>
+        <v>36528.51758101852</v>
       </c>
       <c r="E283" t="n">
         <v>2</v>
@@ -6619,7 +6619,7 @@
         <v>471</v>
       </c>
       <c r="D284" s="2" t="n">
-        <v>36528.63513888889</v>
+        <v>36528.63755787037</v>
       </c>
       <c r="E284" t="n">
         <v>3</v>
@@ -6641,7 +6641,7 @@
         <v>476</v>
       </c>
       <c r="D285" s="2" t="n">
-        <v>36528.51569444445</v>
+        <v>36528.51758101852</v>
       </c>
       <c r="E285" t="n">
         <v>2</v>
@@ -6663,7 +6663,7 @@
         <v>476</v>
       </c>
       <c r="D286" s="2" t="n">
-        <v>36528.64</v>
+        <v>36528.64193287037</v>
       </c>
       <c r="E286" t="n">
         <v>3</v>
@@ -6685,7 +6685,7 @@
         <v>476</v>
       </c>
       <c r="D287" s="2" t="n">
-        <v>36528.64</v>
+        <v>36528.64193287037</v>
       </c>
       <c r="E287" t="n">
         <v>1</v>
@@ -6707,7 +6707,7 @@
         <v>480</v>
       </c>
       <c r="D288" s="2" t="n">
-        <v>36528.52141203704</v>
+        <v>36528.52600694444</v>
       </c>
       <c r="E288" t="n">
         <v>2</v>
@@ -6729,7 +6729,7 @@
         <v>480</v>
       </c>
       <c r="D289" s="2" t="n">
-        <v>36528.73043981481</v>
+        <v>36528.73532407408</v>
       </c>
       <c r="E289" t="n">
         <v>3</v>
@@ -6751,7 +6751,7 @@
         <v>480</v>
       </c>
       <c r="D290" s="2" t="n">
-        <v>36528.73043981481</v>
+        <v>36528.73532407408</v>
       </c>
       <c r="E290" t="n">
         <v>1</v>
@@ -6773,7 +6773,7 @@
         <v>474</v>
       </c>
       <c r="D291" s="2" t="n">
-        <v>36528.56136574074</v>
+        <v>36528.56638888889</v>
       </c>
       <c r="E291" t="n">
         <v>2</v>
@@ -6795,7 +6795,7 @@
         <v>474</v>
       </c>
       <c r="D292" s="2" t="n">
-        <v>36528.77178240741</v>
+        <v>36528.77746527778</v>
       </c>
       <c r="E292" t="n">
         <v>3</v>
@@ -6817,7 +6817,7 @@
         <v>474</v>
       </c>
       <c r="D293" s="2" t="n">
-        <v>36528.77178240741</v>
+        <v>36528.77746527778</v>
       </c>
       <c r="E293" t="n">
         <v>1</v>
@@ -6839,7 +6839,7 @@
         <v>475</v>
       </c>
       <c r="D294" s="2" t="n">
-        <v>36528.58625</v>
+        <v>36528.58936342593</v>
       </c>
       <c r="E294" t="n">
         <v>2</v>
@@ -6861,7 +6861,7 @@
         <v>475</v>
       </c>
       <c r="D295" s="2" t="n">
-        <v>36528.68902777778</v>
+        <v>36528.69273148148</v>
       </c>
       <c r="E295" t="n">
         <v>3</v>
@@ -6883,7 +6883,7 @@
         <v>475</v>
       </c>
       <c r="D296" s="2" t="n">
-        <v>36528.68902777778</v>
+        <v>36528.69273148148</v>
       </c>
       <c r="E296" t="n">
         <v>1</v>
@@ -6905,7 +6905,7 @@
         <v>484</v>
       </c>
       <c r="D297" s="2" t="n">
-        <v>36528.58625</v>
+        <v>36528.58936342593</v>
       </c>
       <c r="E297" t="n">
         <v>2</v>
@@ -6927,7 +6927,7 @@
         <v>484</v>
       </c>
       <c r="D298" s="2" t="n">
-        <v>36528.65847222223</v>
+        <v>36528.66206018518</v>
       </c>
       <c r="E298" t="n">
         <v>3</v>
@@ -6949,7 +6949,7 @@
         <v>469</v>
       </c>
       <c r="D299" s="2" t="n">
-        <v>36528.58694444445</v>
+        <v>36528.59071759259</v>
       </c>
       <c r="E299" t="n">
         <v>2</v>
@@ -6971,7 +6971,7 @@
         <v>469</v>
       </c>
       <c r="D300" s="2" t="n">
-        <v>36528.67236111111</v>
+        <v>36528.67649305556</v>
       </c>
       <c r="E300" t="n">
         <v>3</v>
@@ -6993,7 +6993,7 @@
         <v>469</v>
       </c>
       <c r="D301" s="2" t="n">
-        <v>36528.67236111111</v>
+        <v>36528.67649305556</v>
       </c>
       <c r="E301" t="n">
         <v>1</v>
@@ -7015,7 +7015,7 @@
         <v>481</v>
       </c>
       <c r="D302" s="2" t="n">
-        <v>36528.63513888889</v>
+        <v>36528.63755787037</v>
       </c>
       <c r="E302" t="n">
         <v>2</v>
@@ -7037,7 +7037,7 @@
         <v>481</v>
       </c>
       <c r="D303" s="2" t="n">
-        <v>36528.72888888889</v>
+        <v>36528.73173611111</v>
       </c>
       <c r="E303" t="n">
         <v>3</v>
@@ -7059,7 +7059,7 @@
         <v>481</v>
       </c>
       <c r="D304" s="2" t="n">
-        <v>36528.72888888889</v>
+        <v>36528.73173611111</v>
       </c>
       <c r="E304" t="n">
         <v>1</v>
@@ -7081,7 +7081,7 @@
         <v>476</v>
       </c>
       <c r="D305" s="2" t="n">
-        <v>36528.64</v>
+        <v>36528.64193287037</v>
       </c>
       <c r="E305" t="n">
         <v>2</v>
@@ -7103,7 +7103,7 @@
         <v>476</v>
       </c>
       <c r="D306" s="2" t="n">
-        <v>36528.71916666667</v>
+        <v>36528.72172453703</v>
       </c>
       <c r="E306" t="n">
         <v>3</v>
@@ -7125,7 +7125,7 @@
         <v>476</v>
       </c>
       <c r="D307" s="2" t="n">
-        <v>36528.71916666667</v>
+        <v>36528.72172453703</v>
       </c>
       <c r="E307" t="n">
         <v>1</v>
@@ -7147,7 +7147,7 @@
         <v>476</v>
       </c>
       <c r="D308" s="2" t="n">
-        <v>36528.71916666667</v>
+        <v>36528.72172453703</v>
       </c>
       <c r="E308" t="n">
         <v>2</v>
@@ -7169,7 +7169,7 @@
         <v>476</v>
       </c>
       <c r="D309" s="2" t="n">
-        <v>36528.83305555556</v>
+        <v>36528.83603009259</v>
       </c>
       <c r="E309" t="n">
         <v>3</v>
@@ -7191,7 +7191,7 @@
         <v>469</v>
       </c>
       <c r="D310" s="2" t="n">
-        <v>36528.72888888889</v>
+        <v>36528.73173611111</v>
       </c>
       <c r="E310" t="n">
         <v>2</v>
@@ -7213,7 +7213,7 @@
         <v>469</v>
       </c>
       <c r="D311" s="2" t="n">
-        <v>36528.81916666667</v>
+        <v>36528.82228009259</v>
       </c>
       <c r="E311" t="n">
         <v>3</v>
@@ -7235,7 +7235,7 @@
         <v>481</v>
       </c>
       <c r="D312" s="2" t="n">
-        <v>36528.72888888889</v>
+        <v>36528.73173611111</v>
       </c>
       <c r="E312" t="n">
         <v>2</v>
@@ -7257,7 +7257,7 @@
         <v>481</v>
       </c>
       <c r="D313" s="2" t="n">
-        <v>36528.81916666667</v>
+        <v>36528.82243055556</v>
       </c>
       <c r="E313" t="n">
         <v>3</v>
@@ -7279,7 +7279,7 @@
         <v>481</v>
       </c>
       <c r="D314" s="2" t="n">
-        <v>36528.81916666667</v>
+        <v>36528.82243055556</v>
       </c>
       <c r="E314" t="n">
         <v>1</v>
@@ -7301,7 +7301,7 @@
         <v>483</v>
       </c>
       <c r="D315" s="2" t="n">
-        <v>36528.72974537037</v>
+        <v>36528.73409722222</v>
       </c>
       <c r="E315" t="n">
         <v>2</v>
@@ -7323,7 +7323,7 @@
         <v>483</v>
       </c>
       <c r="D316" s="2" t="n">
-        <v>36529.00613425926</v>
+        <v>36529.01068287037</v>
       </c>
       <c r="E316" t="n">
         <v>3</v>
@@ -7345,7 +7345,7 @@
         <v>483</v>
       </c>
       <c r="D317" s="2" t="n">
-        <v>36529.00613425926</v>
+        <v>36529.01068287037</v>
       </c>
       <c r="E317" t="n">
         <v>1</v>
@@ -7367,7 +7367,7 @@
         <v>486</v>
       </c>
       <c r="D318" s="2" t="n">
-        <v>36528.73043981481</v>
+        <v>36528.73532407408</v>
       </c>
       <c r="E318" t="n">
         <v>2</v>
@@ -7389,7 +7389,7 @@
         <v>486</v>
       </c>
       <c r="D319" s="2" t="n">
-        <v>36528.97835648148</v>
+        <v>36528.98384259259</v>
       </c>
       <c r="E319" t="n">
         <v>3</v>
@@ -7411,7 +7411,7 @@
         <v>486</v>
       </c>
       <c r="D320" s="2" t="n">
-        <v>36528.97835648148</v>
+        <v>36528.98384259259</v>
       </c>
       <c r="E320" t="n">
         <v>1</v>
@@ -7433,7 +7433,7 @@
         <v>480</v>
       </c>
       <c r="D321" s="2" t="n">
-        <v>36528.73043981481</v>
+        <v>36528.73532407408</v>
       </c>
       <c r="E321" t="n">
         <v>2</v>
@@ -7455,7 +7455,7 @@
         <v>480</v>
       </c>
       <c r="D322" s="2" t="n">
-        <v>36528.85891203704</v>
+        <v>36528.86407407407</v>
       </c>
       <c r="E322" t="n">
         <v>3</v>
@@ -7477,7 +7477,7 @@
         <v>474</v>
       </c>
       <c r="D323" s="2" t="n">
-        <v>36528.77178240741</v>
+        <v>36528.77746527778</v>
       </c>
       <c r="E323" t="n">
         <v>2</v>
@@ -7499,7 +7499,7 @@
         <v>474</v>
       </c>
       <c r="D324" s="2" t="n">
-        <v>36528.92594907407</v>
+        <v>36528.93224537037</v>
       </c>
       <c r="E324" t="n">
         <v>3</v>
@@ -7521,7 +7521,7 @@
         <v>474</v>
       </c>
       <c r="D325" s="2" t="n">
-        <v>36528.92594907407</v>
+        <v>36528.93224537037</v>
       </c>
       <c r="E325" t="n">
         <v>1</v>
@@ -7543,7 +7543,7 @@
         <v>474</v>
       </c>
       <c r="D326" s="2" t="n">
-        <v>36528.92594907407</v>
+        <v>36528.93224537037</v>
       </c>
       <c r="E326" t="n">
         <v>2</v>
@@ -7565,7 +7565,7 @@
         <v>474</v>
       </c>
       <c r="D327" s="2" t="n">
-        <v>36529.00094907408</v>
+        <v>36529.0078587963</v>
       </c>
       <c r="E327" t="n">
         <v>3</v>
@@ -7587,7 +7587,7 @@
         <v>472</v>
       </c>
       <c r="D328" s="2" t="n">
-        <v>36528.97835648148</v>
+        <v>36528.98384259259</v>
       </c>
       <c r="E328" t="n">
         <v>2</v>
@@ -7609,7 +7609,7 @@
         <v>472</v>
       </c>
       <c r="D329" s="2" t="n">
-        <v>36529.04641203704</v>
+        <v>36529.05201388889</v>
       </c>
       <c r="E329" t="n">
         <v>3</v>
@@ -7631,7 +7631,7 @@
         <v>486</v>
       </c>
       <c r="D330" s="2" t="n">
-        <v>36529.00094907408</v>
+        <v>36529.0078587963</v>
       </c>
       <c r="E330" t="n">
         <v>2</v>
@@ -7653,7 +7653,7 @@
         <v>486</v>
       </c>
       <c r="D331" s="2" t="n">
-        <v>36529.25025462963</v>
+        <v>36529.25777777778</v>
       </c>
       <c r="E331" t="n">
         <v>3</v>
@@ -7675,7 +7675,7 @@
         <v>486</v>
       </c>
       <c r="D332" s="2" t="n">
-        <v>36529.25025462963</v>
+        <v>36529.25777777778</v>
       </c>
       <c r="E332" t="n">
         <v>1</v>
@@ -7697,7 +7697,7 @@
         <v>481</v>
       </c>
       <c r="D333" s="2" t="n">
-        <v>36529.00613425926</v>
+        <v>36529.01068287037</v>
       </c>
       <c r="E333" t="n">
         <v>2</v>
@@ -7719,7 +7719,7 @@
         <v>481</v>
       </c>
       <c r="D334" s="2" t="n">
-        <v>36529.12974537037</v>
+        <v>36529.13453703704</v>
       </c>
       <c r="E334" t="n">
         <v>3</v>
@@ -7741,7 +7741,7 @@
         <v>483</v>
       </c>
       <c r="D335" s="2" t="n">
-        <v>36529.00613425926</v>
+        <v>36529.01068287037</v>
       </c>
       <c r="E335" t="n">
         <v>2</v>
@@ -7763,7 +7763,7 @@
         <v>483</v>
       </c>
       <c r="D336" s="2" t="n">
-        <v>36529.09918981481</v>
+        <v>36529.10386574074</v>
       </c>
       <c r="E336" t="n">
         <v>3</v>
@@ -7785,7 +7785,7 @@
         <v>483</v>
       </c>
       <c r="D337" s="2" t="n">
-        <v>36529.09918981481</v>
+        <v>36529.10386574074</v>
       </c>
       <c r="E337" t="n">
         <v>1</v>
@@ -7807,7 +7807,7 @@
         <v>475</v>
       </c>
       <c r="D338" s="2" t="n">
-        <v>36529.04641203704</v>
+        <v>36529.05201388889</v>
       </c>
       <c r="E338" t="n">
         <v>2</v>
@@ -7829,7 +7829,7 @@
         <v>475</v>
       </c>
       <c r="D339" s="2" t="n">
-        <v>36529.13252314815</v>
+        <v>36529.13836805556</v>
       </c>
       <c r="E339" t="n">
         <v>3</v>
@@ -7851,7 +7851,7 @@
         <v>483</v>
       </c>
       <c r="D340" s="2" t="n">
-        <v>36529.09918981481</v>
+        <v>36529.10386574074</v>
       </c>
       <c r="E340" t="n">
         <v>2</v>
@@ -7873,7 +7873,7 @@
         <v>483</v>
       </c>
       <c r="D341" s="2" t="n">
-        <v>36529.23391203704</v>
+        <v>36529.23917824074</v>
       </c>
       <c r="E341" t="n">
         <v>3</v>
@@ -7895,7 +7895,7 @@
         <v>486</v>
       </c>
       <c r="D342" s="2" t="n">
-        <v>36529.25025462963</v>
+        <v>36529.25777777778</v>
       </c>
       <c r="E342" t="n">
         <v>2</v>
@@ -7917,7 +7917,7 @@
         <v>486</v>
       </c>
       <c r="D343" s="2" t="n">
-        <v>36529.41344907408</v>
+        <v>36529.42133101852</v>
       </c>
       <c r="E343" t="n">
         <v>3</v>
@@ -7939,7 +7939,7 @@
         <v>486</v>
       </c>
       <c r="D344" s="2" t="n">
-        <v>36529.41344907408</v>
+        <v>36529.42133101852</v>
       </c>
       <c r="E344" t="n">
         <v>1</v>
@@ -7961,7 +7961,7 @@
         <v>486</v>
       </c>
       <c r="D345" s="2" t="n">
-        <v>36529.41344907408</v>
+        <v>36529.42133101852</v>
       </c>
       <c r="E345" t="n">
         <v>2</v>
@@ -7983,7 +7983,7 @@
         <v>486</v>
       </c>
       <c r="D346" s="2" t="n">
-        <v>36529.66344907408</v>
+        <v>36529.67195601852</v>
       </c>
       <c r="E346" t="n">
         <v>3</v>

</xml_diff>